<commit_message>
added more fields for report page
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crchemist/development/donpmm/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEE6BCF-6730-3547-8F59-1FA0F7A1224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9959CB-651B-A048-B514-48ADC78DE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{F811705A-BC7D-E149-A537-E4F41477A2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Донесення" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Донесення!$A$13:$K$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Донесення!$A$1:$K$29</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -369,16 +368,7 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -389,30 +379,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -436,12 +408,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,6 +474,7 @@
       <sheetName val="Реестр шлях.пут."/>
       <sheetName val="Донесення"/>
       <sheetName val="SourceSheet"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -489,6 +489,7 @@
           <cell r="R2" t="str">
             <v>Залишок початок</v>
           </cell>
+          <cell r="X2"/>
         </row>
         <row r="3">
           <cell r="B3" t="str">
@@ -506,11 +507,14 @@
           <cell r="G3" t="str">
             <v>К. Ісмаїлов</v>
           </cell>
+          <cell r="R3"/>
+          <cell r="X3"/>
         </row>
         <row r="4">
           <cell r="R4" t="str">
             <v>6307E6</v>
           </cell>
+          <cell r="X4"/>
         </row>
         <row r="5">
           <cell r="B5" t="str">
@@ -613,6 +617,7 @@
           <cell r="D7">
             <v>3</v>
           </cell>
+          <cell r="E7"/>
           <cell r="F7">
             <v>4</v>
           </cell>
@@ -675,6 +680,10 @@
           <cell r="R8">
             <v>8123</v>
           </cell>
+          <cell r="S8"/>
+          <cell r="T8"/>
+          <cell r="U8"/>
+          <cell r="X8"/>
         </row>
         <row r="9">
           <cell r="J9">
@@ -743,6 +752,10 @@
           <cell r="R12">
             <v>3232</v>
           </cell>
+          <cell r="S12"/>
+          <cell r="T12"/>
+          <cell r="U12"/>
+          <cell r="X12"/>
         </row>
         <row r="13">
           <cell r="B13" t="str">
@@ -836,9 +849,11 @@
           <cell r="B15">
             <v>5</v>
           </cell>
+          <cell r="C15"/>
           <cell r="D15">
             <v>6</v>
           </cell>
+          <cell r="E15"/>
           <cell r="F15">
             <v>7</v>
           </cell>
@@ -901,6 +916,10 @@
           <cell r="R16">
             <v>88888</v>
           </cell>
+          <cell r="S16"/>
+          <cell r="T16"/>
+          <cell r="U16"/>
+          <cell r="X16"/>
         </row>
         <row r="17">
           <cell r="J17">
@@ -969,6 +988,10 @@
           <cell r="R20">
             <v>6666</v>
           </cell>
+          <cell r="S20"/>
+          <cell r="T20"/>
+          <cell r="U20"/>
+          <cell r="X20"/>
         </row>
         <row r="21">
           <cell r="J21">
@@ -1037,6 +1060,10 @@
           <cell r="R24" t="str">
             <v>fj99</v>
           </cell>
+          <cell r="S24"/>
+          <cell r="T24"/>
+          <cell r="U24"/>
+          <cell r="X24"/>
         </row>
         <row r="25">
           <cell r="J25">
@@ -1105,6 +1132,10 @@
           <cell r="R28">
             <v>777</v>
           </cell>
+          <cell r="S28"/>
+          <cell r="T28"/>
+          <cell r="U28"/>
+          <cell r="X28"/>
         </row>
         <row r="29">
           <cell r="J29">
@@ -1173,6 +1204,10 @@
           <cell r="R32" t="str">
             <v>8888A2</v>
           </cell>
+          <cell r="S32"/>
+          <cell r="T32"/>
+          <cell r="U32"/>
+          <cell r="X32"/>
         </row>
         <row r="33">
           <cell r="J33">
@@ -1241,6 +1276,10 @@
           <cell r="R36" t="str">
             <v>999nine</v>
           </cell>
+          <cell r="S36"/>
+          <cell r="T36"/>
+          <cell r="U36"/>
+          <cell r="X36"/>
         </row>
         <row r="37">
           <cell r="J37">
@@ -1309,6 +1348,10 @@
           <cell r="R40">
             <v>1010</v>
           </cell>
+          <cell r="S40"/>
+          <cell r="T40"/>
+          <cell r="U40"/>
+          <cell r="X40"/>
         </row>
         <row r="41">
           <cell r="J41">
@@ -1377,6 +1420,10 @@
           <cell r="R44" t="str">
             <v>111!</v>
           </cell>
+          <cell r="S44"/>
+          <cell r="T44"/>
+          <cell r="U44"/>
+          <cell r="X44"/>
         </row>
         <row r="45">
           <cell r="J45">
@@ -1445,6 +1492,10 @@
           <cell r="R48">
             <v>1212</v>
           </cell>
+          <cell r="S48"/>
+          <cell r="T48"/>
+          <cell r="U48"/>
+          <cell r="X48"/>
         </row>
         <row r="49">
           <cell r="J49">
@@ -1513,6 +1564,10 @@
           <cell r="R52">
             <v>1313</v>
           </cell>
+          <cell r="S52"/>
+          <cell r="T52"/>
+          <cell r="U52"/>
+          <cell r="X52"/>
         </row>
         <row r="53">
           <cell r="J53">
@@ -1581,6 +1636,10 @@
           <cell r="R56">
             <v>1414</v>
           </cell>
+          <cell r="S56"/>
+          <cell r="T56"/>
+          <cell r="U56"/>
+          <cell r="X56"/>
         </row>
         <row r="57">
           <cell r="J57">
@@ -1649,6 +1708,10 @@
           <cell r="R60">
             <v>1515</v>
           </cell>
+          <cell r="S60"/>
+          <cell r="T60"/>
+          <cell r="U60"/>
+          <cell r="X60"/>
         </row>
         <row r="61">
           <cell r="J61">
@@ -1717,6 +1780,10 @@
           <cell r="R64">
             <v>1616</v>
           </cell>
+          <cell r="S64"/>
+          <cell r="T64"/>
+          <cell r="U64"/>
+          <cell r="X64"/>
         </row>
         <row r="65">
           <cell r="J65">
@@ -1785,6 +1852,10 @@
           <cell r="R68">
             <v>1718</v>
           </cell>
+          <cell r="S68"/>
+          <cell r="T68"/>
+          <cell r="U68"/>
+          <cell r="X68"/>
         </row>
         <row r="69">
           <cell r="J69">
@@ -1853,6 +1924,10 @@
           <cell r="R72">
             <v>1818</v>
           </cell>
+          <cell r="S72"/>
+          <cell r="T72"/>
+          <cell r="U72"/>
+          <cell r="X72"/>
         </row>
         <row r="73">
           <cell r="J73">
@@ -1921,6 +1996,10 @@
           <cell r="R76">
             <v>2020</v>
           </cell>
+          <cell r="S76"/>
+          <cell r="T76"/>
+          <cell r="U76"/>
+          <cell r="X76"/>
         </row>
         <row r="77">
           <cell r="J77">
@@ -1989,6 +2068,10 @@
           <cell r="R80">
             <v>2121</v>
           </cell>
+          <cell r="S80"/>
+          <cell r="T80"/>
+          <cell r="U80"/>
+          <cell r="X80"/>
         </row>
         <row r="81">
           <cell r="J81">
@@ -2057,6 +2140,10 @@
           <cell r="R84">
             <v>2222</v>
           </cell>
+          <cell r="S84"/>
+          <cell r="T84"/>
+          <cell r="U84"/>
+          <cell r="X84"/>
         </row>
         <row r="85">
           <cell r="J85">
@@ -2118,6 +2205,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="88">
+          <cell r="J88"/>
+          <cell r="R88"/>
+          <cell r="S88"/>
+          <cell r="T88"/>
+          <cell r="U88"/>
+          <cell r="X88"/>
+        </row>
         <row r="89">
           <cell r="J89">
             <v>345</v>
@@ -2178,6 +2273,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="92">
+          <cell r="J92"/>
+          <cell r="R92"/>
+          <cell r="S92"/>
+          <cell r="T92"/>
+          <cell r="U92"/>
+          <cell r="X92"/>
+        </row>
         <row r="93">
           <cell r="J93">
             <v>345</v>
@@ -2238,6 +2341,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="96">
+          <cell r="J96"/>
+          <cell r="R96"/>
+          <cell r="S96"/>
+          <cell r="T96"/>
+          <cell r="U96"/>
+          <cell r="X96"/>
+        </row>
         <row r="97">
           <cell r="J97">
             <v>345</v>
@@ -2298,6 +2409,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="100">
+          <cell r="J100"/>
+          <cell r="R100"/>
+          <cell r="S100"/>
+          <cell r="T100"/>
+          <cell r="U100"/>
+          <cell r="X100"/>
+        </row>
         <row r="101">
           <cell r="J101">
             <v>345</v>
@@ -2358,6 +2477,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="104">
+          <cell r="J104"/>
+          <cell r="R104"/>
+          <cell r="S104"/>
+          <cell r="T104"/>
+          <cell r="U104"/>
+          <cell r="X104"/>
+        </row>
         <row r="105">
           <cell r="J105">
             <v>345</v>
@@ -2418,6 +2545,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="108">
+          <cell r="J108"/>
+          <cell r="R108"/>
+          <cell r="S108"/>
+          <cell r="T108"/>
+          <cell r="U108"/>
+          <cell r="X108"/>
+        </row>
         <row r="109">
           <cell r="J109">
             <v>345</v>
@@ -2478,6 +2613,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="112">
+          <cell r="J112"/>
+          <cell r="R112"/>
+          <cell r="S112"/>
+          <cell r="T112"/>
+          <cell r="U112"/>
+          <cell r="X112"/>
+        </row>
         <row r="113">
           <cell r="J113">
             <v>345</v>
@@ -2538,6 +2681,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="116">
+          <cell r="J116"/>
+          <cell r="R116"/>
+          <cell r="S116"/>
+          <cell r="T116"/>
+          <cell r="U116"/>
+          <cell r="X116"/>
+        </row>
         <row r="117">
           <cell r="J117">
             <v>345</v>
@@ -2598,6 +2749,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="120">
+          <cell r="J120"/>
+          <cell r="R120"/>
+          <cell r="S120"/>
+          <cell r="T120"/>
+          <cell r="U120"/>
+          <cell r="X120"/>
+        </row>
         <row r="121">
           <cell r="J121">
             <v>345</v>
@@ -2658,6 +2817,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="124">
+          <cell r="J124"/>
+          <cell r="R124"/>
+          <cell r="S124"/>
+          <cell r="T124"/>
+          <cell r="U124"/>
+          <cell r="X124"/>
+        </row>
         <row r="125">
           <cell r="J125">
             <v>345</v>
@@ -2718,6 +2885,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="128">
+          <cell r="J128"/>
+          <cell r="R128"/>
+          <cell r="S128"/>
+          <cell r="T128"/>
+          <cell r="U128"/>
+          <cell r="X128"/>
+        </row>
         <row r="129">
           <cell r="J129">
             <v>345</v>
@@ -2778,6 +2953,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="132">
+          <cell r="J132"/>
+          <cell r="R132"/>
+          <cell r="S132"/>
+          <cell r="T132"/>
+          <cell r="U132"/>
+          <cell r="X132"/>
+        </row>
         <row r="133">
           <cell r="J133">
             <v>345</v>
@@ -2838,6 +3021,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="136">
+          <cell r="J136"/>
+          <cell r="R136"/>
+          <cell r="S136"/>
+          <cell r="T136"/>
+          <cell r="U136"/>
+          <cell r="X136"/>
+        </row>
         <row r="137">
           <cell r="J137">
             <v>345</v>
@@ -2898,6 +3089,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="140">
+          <cell r="J140"/>
+          <cell r="R140"/>
+          <cell r="S140"/>
+          <cell r="T140"/>
+          <cell r="U140"/>
+          <cell r="X140"/>
+        </row>
         <row r="141">
           <cell r="J141">
             <v>345</v>
@@ -2958,6 +3157,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="144">
+          <cell r="J144"/>
+          <cell r="R144"/>
+          <cell r="S144"/>
+          <cell r="T144"/>
+          <cell r="U144"/>
+          <cell r="X144"/>
+        </row>
         <row r="145">
           <cell r="J145">
             <v>345</v>
@@ -3018,6 +3225,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="148">
+          <cell r="J148"/>
+          <cell r="R148"/>
+          <cell r="S148"/>
+          <cell r="T148"/>
+          <cell r="U148"/>
+          <cell r="X148"/>
+        </row>
         <row r="149">
           <cell r="J149">
             <v>345</v>
@@ -3028,6 +3243,7 @@
           <cell r="S149">
             <v>111</v>
           </cell>
+          <cell r="T149"/>
           <cell r="U149">
             <v>3</v>
           </cell>
@@ -3075,6 +3291,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="152">
+          <cell r="J152"/>
+          <cell r="R152"/>
+          <cell r="S152"/>
+          <cell r="T152"/>
+          <cell r="U152"/>
+          <cell r="X152"/>
+        </row>
         <row r="153">
           <cell r="J153">
             <v>345</v>
@@ -3135,6 +3359,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="156">
+          <cell r="J156"/>
+          <cell r="R156"/>
+          <cell r="S156"/>
+          <cell r="T156"/>
+          <cell r="U156"/>
+          <cell r="X156"/>
+        </row>
         <row r="157">
           <cell r="J157">
             <v>345</v>
@@ -3195,6 +3427,14 @@
             <v>ДП-з-Євро5 В0</v>
           </cell>
         </row>
+        <row r="160">
+          <cell r="J160"/>
+          <cell r="R160"/>
+          <cell r="S160"/>
+          <cell r="T160"/>
+          <cell r="U160"/>
+          <cell r="X160"/>
+        </row>
         <row r="161">
           <cell r="J161">
             <v>345</v>
@@ -3256,6 +3496,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3562,279 +3803,276 @@
   <dimension ref="A1:O105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="D6" sqref="D6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" style="2" customWidth="1"/>
-    <col min="14" max="15" width="8.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="14.5" style="2"/>
+    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="8.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
-    <row r="2" spans="1:15" ht="12.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:15" ht="15" customHeight="1">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="21" t="str">
         <f>" за період з " &amp;TEXT( VALUE([1]SourceSheet!C3), "dd.mm.YYYY") &amp; " по " &amp; TEXT( VALUE([1]SourceSheet!D3), "dd.mm.YYYY")  &amp;" року"</f>
         <v xml:space="preserve"> за період з 21.03.2023 по 23.04.2023 року</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="M4" s="5"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="4.5" customHeight="1">
-      <c r="A5" s="6"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="5"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="51.75" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="22"/>
+      <c r="J7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="10"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f>[1]SourceSheet!B3</f>
-        <v>БМТЗ РМЗ</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="L8" s="10"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:15" ht="6.75" customHeight="1" thickBot="1">
-      <c r="A9" s="14"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="16" t="str">
+      <c r="D10" s="26" t="str">
         <f>"перебувало на початок звітнього періоду(" &amp; TEXT( VALUE([1]SourceSheet!C3), "dd.mm.YY") &amp; ")"</f>
         <v>перебувало на початок звітнього періоду(21.03.23)</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="16" t="str">
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26" t="str">
         <f>"наявність станом на (" &amp; TEXT( VALUE([1]SourceSheet!D3), "dd.mm.YY")  &amp; ")"</f>
         <v>наявність станом на (23.04.23)</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:15" ht="91.5" customHeight="1" thickBot="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="19" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="21">
+      <c r="A12" s="12">
         <v>1</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="13">
         <v>2</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="13">
         <v>3</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="13">
         <v>5</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="13">
         <v>6</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="13">
         <v>7</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="13">
         <v>9</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="13">
         <v>11</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="13">
         <v>12</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="13">
         <v>13</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="13">
         <v>14</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:15" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A13" s="21">
+      <c r="A13" s="12">
         <v>1</v>
       </c>
-      <c r="B13" s="21" t="str" cm="1">
+      <c r="B13" s="12" t="str" cm="1">
         <f t="array" ref="B13:B15">_xlfn.LET(
     _xlpm.data,_xlfn.VSTACK([1]SourceSheet!X5:X163, [1]SourceSheet!Y5:Y163),
     _xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.data,_xlpm.data&lt;&gt;""))
 )</f>
         <v>ДП-л-Євро5 В0</v>
       </c>
-      <c r="C13" s="21" t="str">
+      <c r="C13" s="12" t="str">
         <f t="shared" ref="C13:C22" si="0">IF(ISBLANK(B13), "", "л/кг")</f>
         <v>л/кг</v>
       </c>
-      <c r="D13" s="21" t="str" cm="1">
+      <c r="D13" s="12" t="str" cm="1">
         <f t="array" ref="D13">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B13),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -3845,7 +4083,7 @@
     )</f>
         <v>40/34</v>
       </c>
-      <c r="E13" s="21" t="str">
+      <c r="E13" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B13,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B13, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B13, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3853,9 +4091,9 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="F13" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B13,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B13, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B13, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3863,9 +4101,9 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="G13" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="12" t="e">
         <f t="shared" ref="G13:G22" si="1">_xlfn.LET(
     _xlpm.ltrsOwn, IF(OR(LEN(E13)=0,ISBLANK(E13)),
         0, _xlfn.TEXTBEFORE(E13, "/")),
@@ -3877,9 +4115,9 @@
         0, _xlfn.TEXTAFTER(F13, "/")),
     IF(ISBLANK($B13), "", _xlpm.ltrsOwn+_xlpm.ltrsOther &amp; "/" &amp; _xlpm.kgsOwn+_xlpm.kgsOther)
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="H13" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H13" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B13,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B13, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B13, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3887,13 +4125,13 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>120/101</v>
-      </c>
-      <c r="I13" s="24" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I13" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B13, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B13, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B13), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B13, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B13, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v>22/18</v>
       </c>
-      <c r="J13" s="21" t="str">
+      <c r="J13" s="12" t="e">
         <f>_xlfn.LET(
     _xlpm.ltrsOwn, IF(OR(LEN(H13)=0,ISBLANK(H13)),
         0, _xlfn.TEXTBEFORE(H13, "/")),
@@ -3905,9 +4143,9 @@
         0, _xlfn.TEXTAFTER(I13, "/")),
     IF(ISBLANK($B13), "", _xlpm.ltrsOther+_xlpm.ltrsOwn &amp; "/" &amp; _xlpm.kgsOwn+_xlpm.kgsOther)
 )</f>
-        <v>142/119</v>
-      </c>
-      <c r="K13" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="12" t="e">
         <f>_xlfn.LET(
     _xlpm.ltrsBefore, IF(OR(LEN(D13)=0,ISBLANK(D13)),
         0, _xlfn.TEXTBEFORE(D13, "/")),
@@ -3923,25 +4161,25 @@
         0, _xlfn.TEXTAFTER(J13, "/")),
     IF(ISBLANK($B13), "", (_xlpm.ltrsBefore+_xlpm.ltrsIncome- _xlpm.ltrsOutcome) &amp; "/" &amp; (_xlpm.kgsBefore + _xlpm.kgsIncome - _xlpm.kgsOutcome ))
 )</f>
-        <v>-102/-85</v>
-      </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A14" s="21">
+      <c r="A14" s="12">
         <v>2</v>
       </c>
-      <c r="B14" s="21" t="str">
+      <c r="B14" s="12" t="str">
         <v>ДП-з-Євро5 В0</v>
       </c>
-      <c r="C14" s="21" t="str">
+      <c r="C14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>л/кг</v>
       </c>
-      <c r="D14" s="21" t="str" cm="1">
+      <c r="D14" s="12" t="str" cm="1">
         <f t="array" ref="D14">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B14),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -3952,7 +4190,7 @@
     )</f>
         <v>0/0</v>
       </c>
-      <c r="E14" s="21" t="str">
+      <c r="E14" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B14,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B14, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B14, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3960,9 +4198,9 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="F14" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B14,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B14, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B14, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3970,13 +4208,13 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="G14" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G14" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>0/0</v>
-      </c>
-      <c r="H14" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B14,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B14, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B14, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -3984,13 +4222,13 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>560/476</v>
-      </c>
-      <c r="I14" s="24" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I14" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B14, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B14, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B14), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B14, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B14, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v>23/20</v>
       </c>
-      <c r="J14" s="21" t="str">
+      <c r="J14" s="12" t="e">
         <f t="shared" ref="J14:J22" si="2">_xlfn.LET(
     _xlpm.ltrsOwn, IF(OR(LEN(H14)=0,ISBLANK(H14)),
         0, _xlfn.TEXTBEFORE(H14, "/")),
@@ -4002,9 +4240,9 @@
         0, _xlfn.TEXTAFTER(I14, "/")),
     IF(ISBLANK($B14), "", _xlpm.ltrsOther+_xlpm.ltrsOwn &amp; "/" &amp; _xlpm.kgsOwn+_xlpm.kgsOther)
 )</f>
-        <v>583/496</v>
-      </c>
-      <c r="K14" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" s="12" t="e">
         <f t="shared" ref="K14:K22" si="3">_xlfn.LET(
     _xlpm.ltrsBefore, IF(OR(LEN(D14)=0,ISBLANK(D14)),
         0, _xlfn.TEXTBEFORE(D14, "/")),
@@ -4020,25 +4258,25 @@
         0, _xlfn.TEXTAFTER(J14, "/")),
     IF(ISBLANK($B14), "", (_xlpm.ltrsBefore+_xlpm.ltrsIncome- _xlpm.ltrsOutcome) &amp; "/" &amp; (_xlpm.kgsBefore + _xlpm.kgsIncome - _xlpm.kgsOutcome ))
 )</f>
-        <v>-583/-496</v>
-      </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A15" s="21">
+      <c r="A15" s="12">
         <v>3</v>
       </c>
-      <c r="B15" s="21" t="str">
+      <c r="B15" s="12" t="str">
         <v>А-80</v>
       </c>
-      <c r="C15" s="21" t="str">
+      <c r="C15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>л/кг</v>
       </c>
-      <c r="D15" s="21" t="str" cm="1">
+      <c r="D15" s="12" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B15),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4049,7 +4287,7 @@
     )</f>
         <v>0/0</v>
       </c>
-      <c r="E15" s="21" t="str">
+      <c r="E15" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B15,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B15, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B15, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4057,9 +4295,9 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>113/85</v>
-      </c>
-      <c r="F15" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B15,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B15, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B15, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4067,13 +4305,13 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>5/4</v>
-      </c>
-      <c r="G15" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>118/89</v>
-      </c>
-      <c r="H15" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H15" s="12" t="e">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B15,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B15, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B15, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4081,35 +4319,35 @@
         _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.kgs,0)
     )
 )</f>
-        <v>0/0</v>
-      </c>
-      <c r="I15" s="24" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B15, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B15, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B15), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B15, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B15, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v>26/20</v>
       </c>
-      <c r="J15" s="21" t="str">
+      <c r="J15" s="12" t="e">
         <f t="shared" si="2"/>
-        <v>26/20</v>
-      </c>
-      <c r="K15" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="12" t="e">
         <f t="shared" si="3"/>
-        <v>92/69</v>
-      </c>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
     </row>
     <row r="16" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A16" s="21">
+      <c r="A16" s="12">
         <v>4</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21" t="str">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D16" s="21" t="str" cm="1">
+      <c r="D16" s="12" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B16),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4120,7 +4358,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E16" s="21" t="str">
+      <c r="E16" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B16,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B16, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B16, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4130,7 +4368,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F16" s="21" t="str">
+      <c r="F16" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B16,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B16, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B16, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4140,11 +4378,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G16" s="21" t="str">
+      <c r="G16" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H16" s="21" t="str">
+      <c r="H16" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B16,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B16, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B16, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4154,33 +4392,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I16" s="24" t="str">
+      <c r="I16" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B16, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B16, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B16), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B16, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B16, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J16" s="21" t="str">
+      <c r="J16" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="21" t="str">
+      <c r="K16" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A17" s="21">
+      <c r="A17" s="12">
         <v>5</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21" t="str">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D17" s="21" t="str" cm="1">
+      <c r="D17" s="12" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B17),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4191,7 +4429,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E17" s="21" t="str">
+      <c r="E17" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B17,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B17, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B17, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4201,7 +4439,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F17" s="21" t="str">
+      <c r="F17" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B17,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B17, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B17, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4211,11 +4449,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G17" s="21" t="str">
+      <c r="G17" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H17" s="21" t="str">
+      <c r="H17" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B17,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B17, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B17, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4225,33 +4463,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I17" s="24" t="str">
+      <c r="I17" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B17, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B17, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B17), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B17, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B17, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J17" s="21" t="str">
+      <c r="J17" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K17" s="21" t="str">
+      <c r="K17" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
     </row>
     <row r="18" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A18" s="21">
+      <c r="A18" s="12">
         <v>6</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21" t="str">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D18" s="21" t="str" cm="1">
+      <c r="D18" s="12" t="str" cm="1">
         <f t="array" ref="D18">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B18),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4262,7 +4500,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E18" s="21" t="str">
+      <c r="E18" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B18,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B18, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B18, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4272,7 +4510,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F18" s="21" t="str">
+      <c r="F18" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B18,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B18, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B18, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4282,11 +4520,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G18" s="21" t="str">
+      <c r="G18" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H18" s="21" t="str">
+      <c r="H18" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B18,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B18, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B18, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4296,33 +4534,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I18" s="24" t="str">
+      <c r="I18" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B18, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B18, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B18), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B18, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B18, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J18" s="21" t="str">
+      <c r="J18" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K18" s="21" t="str">
+      <c r="K18" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A19" s="21">
+      <c r="A19" s="12">
         <v>7</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21" t="str">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D19" s="21" t="str" cm="1">
+      <c r="D19" s="12" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B19),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4333,7 +4571,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E19" s="21" t="str">
+      <c r="E19" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B19,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B19, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B19, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4343,7 +4581,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F19" s="21" t="str">
+      <c r="F19" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B19,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B19, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B19, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4353,11 +4591,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G19" s="21" t="str">
+      <c r="G19" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H19" s="21" t="str">
+      <c r="H19" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B19,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B19, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B19, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4367,33 +4605,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I19" s="24" t="str">
+      <c r="I19" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B19, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B19, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B19), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B19, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B19, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J19" s="21" t="str">
+      <c r="J19" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K19" s="21" t="str">
+      <c r="K19" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A20" s="21">
+      <c r="A20" s="12">
         <v>8</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21" t="str">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D20" s="21" t="str" cm="1">
+      <c r="D20" s="12" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B20),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4404,7 +4642,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E20" s="21" t="str">
+      <c r="E20" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B20,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B20, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B20, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4414,7 +4652,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F20" s="21" t="str">
+      <c r="F20" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B20,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B20, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B20, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4424,11 +4662,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G20" s="21" t="str">
+      <c r="G20" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H20" s="21" t="str">
+      <c r="H20" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B20,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B20, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B20, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4438,33 +4676,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I20" s="24" t="str">
+      <c r="I20" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B20, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B20, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B20), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B20, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B20, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J20" s="21" t="str">
+      <c r="J20" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K20" s="21" t="str">
+      <c r="K20" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
     </row>
     <row r="21" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A21" s="21">
+      <c r="A21" s="12">
         <v>9</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21" t="str">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D21" s="21" t="str" cm="1">
+      <c r="D21" s="12" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B21),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4475,7 +4713,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E21" s="21" t="str">
+      <c r="E21" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B21,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B21, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B21, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4485,7 +4723,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F21" s="21" t="str">
+      <c r="F21" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B21,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B21, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B21, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4495,11 +4733,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G21" s="21" t="str">
+      <c r="G21" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H21" s="21" t="str">
+      <c r="H21" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B21,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B21, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B21, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4509,33 +4747,33 @@
 )</f>
         <v/>
       </c>
-      <c r="I21" s="24" t="str">
+      <c r="I21" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B21, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B21, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B21), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B21, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B21, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J21" s="21" t="str">
+      <c r="J21" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K21" s="21" t="str">
+      <c r="K21" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
     </row>
     <row r="22" spans="1:15" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A22" s="21">
+      <c r="A22" s="12">
         <v>10</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21" t="str">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D22" s="21" t="str" cm="1">
+      <c r="D22" s="12" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.LET(_xlpm.ltrs,
     SUMPRODUCT(
         --(MOD(ROW([1]SourceSheet!$R$2:$R$163)-ROW([1]SourceSheet!$R$2)+1,4)=0),--([1]SourceSheet!$X$2:$X$163=B22),--([1]SourceSheet!$X$2:$X$163&lt;&gt;""),[1]SourceSheet!$R$2:$R$163),
@@ -4546,7 +4784,7 @@
     )</f>
         <v/>
       </c>
-      <c r="E22" s="21" t="str">
+      <c r="E22" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B22,[1]SourceSheet!$S$5:$S$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B22, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B22, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4556,7 +4794,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F22" s="21" t="str">
+      <c r="F22" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$Y$5:$Y$163,B22,[1]SourceSheet!$T$5:$T$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B22, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B22, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4566,11 +4804,11 @@
 )</f>
         <v/>
       </c>
-      <c r="G22" s="21" t="str">
+      <c r="G22" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H22" s="21" t="str">
+      <c r="H22" s="12" t="str">
         <f>_xlfn.LET(_xlpm.ltrs,
     SUMIF([1]SourceSheet!$X$5:$X$163,B22,[1]SourceSheet!$U$5:$U$163),
     _xlpm.kgs, _xlpm.ltrs * IFERROR(HLOOKUP(B22, [1]SourceSheet!$B$5:$I$6,2, FALSE()), HLOOKUP(B22, [1]SourceSheet!$B$13:$I$15,2, FALSE())),
@@ -4580,111 +4818,111 @@
 )</f>
         <v/>
       </c>
-      <c r="I22" s="24" t="str">
+      <c r="I22" s="15" t="str">
         <f>_xlfn.LET(_xlpm.ltrs, IFERROR(HLOOKUP(B22, [1]SourceSheet!$B$5:$I$8,4, FALSE()), HLOOKUP(B22, [1]SourceSheet!$B$13:$I$16,4, FALSE())), IF( ISBLANK(B22), "", _xlpm.ltrs &amp; "/" &amp; ROUND(_xlpm.ltrs * IFERROR(HLOOKUP(B22, [1]SourceSheet!$B$5:$I$8,2, FALSE()), HLOOKUP(B22, [1]SourceSheet!$B$13:$I$16,2, FALSE())),0)))</f>
         <v/>
       </c>
-      <c r="J22" s="21" t="str">
+      <c r="J22" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K22" s="21" t="str">
+      <c r="K22" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A24" s="26" t="str">
+      <c r="A24" s="29" t="str">
         <f t="array" ref="A24">_xlfn.TEXTJOIN(", ", TRUE(), _xlfn._xlws.FILTER([1]SourceSheet!$J$5:$J$163,MOD(_xlfn.SEQUENCE(ROWS([1]SourceSheet!$J$5:$J$163)),4)&lt;&gt;0, FALSE()))</f>
         <v>345, 99, 888, 345, 99, 888, 347, 119, 888, 345, 99, 888, 345, 99, 8, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 88, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888, 345, 99, 888</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:15" ht="18" customHeight="1">
-      <c r="A25" s="26" t="e" cm="1">
+      <c r="A25" s="29" t="e" cm="1">
         <f t="array" aca="1" ref="A25" ca="1">_xlfn.LET(_xlpm.cnt, COUNT(_xlfn._xlws.FILTER([1]SourceSheet!$J$5:$J$163,MOD(_xlfn.SEQUENCE(ROWS([1]SourceSheet!$J$5:$J$163)),4)&lt;&gt;0,FALSE())), "(" &amp; NumberText(_xlpm.cnt) &amp; ") " &amp; _xlpm.cnt &amp; " штук.")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:15" ht="18" customHeight="1">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
     </row>
     <row r="27" spans="1:15" ht="30" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
     </row>
     <row r="28" spans="1:15" ht="18" customHeight="1">
-      <c r="A28" s="27" t="str">
+      <c r="A28" s="28" t="str">
         <f>"Командир " &amp; [1]SourceSheet!B3</f>
         <v>Командир БМТЗ РМЗ</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="E28" s="28" t="str">
+      <c r="B28" s="28"/>
+      <c r="E28" s="17" t="str">
         <f>[1]SourceSheet!F3&amp; "_________________"&amp;[1]SourceSheet!G3</f>
         <v>к-н_________________К. Ісмаїлов</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="12" customHeight="1">
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:15" ht="12" customHeight="1"/>
     <row r="31" spans="1:15" ht="12" customHeight="1"/>
@@ -4692,7 +4930,7 @@
     <row r="33" spans="1:5" ht="12" customHeight="1"/>
     <row r="34" spans="1:5" ht="12" customHeight="1"/>
     <row r="35" spans="1:5" ht="12" customHeight="1">
-      <c r="A35" s="29"/>
+      <c r="A35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="12" customHeight="1"/>
     <row r="37" spans="1:5" ht="12" customHeight="1"/>
@@ -4703,7 +4941,7 @@
     <row r="42" spans="1:5" ht="12" customHeight="1"/>
     <row r="43" spans="1:5" ht="12" customHeight="1"/>
     <row r="44" spans="1:5" ht="12" customHeight="1">
-      <c r="E44" s="23"/>
+      <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:5" ht="12" customHeight="1"/>
     <row r="46" spans="1:5" ht="12" customHeight="1"/>
@@ -4768,12 +5006,12 @@
     <row r="105" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="K10:K11"/>
     <mergeCell ref="A23:K23"/>
     <mergeCell ref="A24:K24"/>
     <mergeCell ref="A25:K25"/>
     <mergeCell ref="A26:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A10:A11"/>
@@ -4782,7 +5020,6 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:K11"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -4793,20 +5030,9 @@
     <mergeCell ref="D6:E7"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.45972222222222198" right="0.34027777777777801" top="0.359722222222222" bottom="0.35" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33A1960-4674-2642-A8F4-22FF6C13335B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>